<commit_message>
fixed some macro stuff
</commit_message>
<xml_diff>
--- a/Test_cases.xlsx
+++ b/Test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parsa_orodes/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parsa_orodes/Documents/COSC202/andie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF4759-07EA-9743-A3B0-A6BE4563CCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9728BF27-551C-2345-BF4B-5C165BCBD170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28780" windowHeight="16600" xr2:uid="{BBDFDA9F-B308-46BA-990B-95E2222DDB26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
   <si>
     <t>Project Name</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t xml:space="preserve">The image and its operations are kept on the panel but the language is changed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw mouse selected area </t>
   </si>
 </sst>
 </file>
@@ -426,14 +429,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -887,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142439C2-4A4F-4125-A1B1-034AF03278CF}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -903,24 +906,24 @@
   <sheetData>
     <row r="1" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:16" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -1085,7 +1088,7 @@
       <c r="G16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1233,7 +1236,9 @@
       <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
@@ -1332,7 +1337,7 @@
         <v>81</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updating the test file
</commit_message>
<xml_diff>
--- a/Test_cases.xlsx
+++ b/Test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parsa_orodes/Documents/COSC202/andie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83128965-2A59-D64F-962F-37F2B66C4427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0F7EC9-C3C6-B74F-AD07-AA44A47C1158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28780" windowHeight="16600" xr2:uid="{BBDFDA9F-B308-46BA-990B-95E2222DDB26}"/>
   </bookViews>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142439C2-4A4F-4125-A1B1-034AF03278CF}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>